<commit_message>
Heatmap and cell abundance profile
</commit_message>
<xml_diff>
--- a/R_C14_rates calculation/0_init_files/colours_cycle.xlsx
+++ b/R_C14_rates calculation/0_init_files/colours_cycle.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deniseong/Documents/GitHub/TAN1810_C14/R_C14_rates calculation/0_init_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E32777-9942-E949-8C1E-89DC13564B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D92A4F-8062-DA4C-8632-E6DE9CD40050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" activeTab="3" xr2:uid="{9959AD80-3573-194E-BAC2-C518CF80D496}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19120" xr2:uid="{9959AD80-3573-194E-BAC2-C518CF80D496}"/>
   </bookViews>
   <sheets>
     <sheet name="cycle" sheetId="1" r:id="rId1"/>
@@ -132,12 +132,6 @@
     <t>#99F8FF</t>
   </si>
   <si>
-    <t>#3299FF</t>
-  </si>
-  <si>
-    <t>#002AFF</t>
-  </si>
-  <si>
     <t>SA-Sc</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>Subantarctic</t>
+  </si>
+  <si>
+    <t>#0D47A1</t>
+  </si>
+  <si>
+    <t>#2196F3</t>
   </si>
 </sst>
 </file>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245E3022-FA4C-1649-9F6C-42EECD9F5BD9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -555,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -780,7 +780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B880A4-5A05-2041-BF2C-5C9A45F67A87}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -796,7 +796,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -820,7 +820,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>

</xml_diff>